<commit_message>
add week 6 tasks
</commit_message>
<xml_diff>
--- a/table_students_is_20_21.xlsx
+++ b/table_students_is_20_21.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vesel\Desktop\IP_IS_2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3D51268D-6A8F-422C-9DFD-1FEB7BDF0F8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB9A0A51-8E31-4F98-A73C-39231C16AAB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7F4C49BC-1414-437F-8268-9DACF2B55AFA}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="70">
   <si>
     <t>Име</t>
   </si>
@@ -67,9 +66,6 @@
     <t>Александров</t>
   </si>
   <si>
-    <t>Чубриев</t>
-  </si>
-  <si>
     <t>Митков</t>
   </si>
   <si>
@@ -82,15 +78,6 @@
     <t>Мустафа</t>
   </si>
   <si>
-    <t>Анжелина</t>
-  </si>
-  <si>
-    <t>Пламенова</t>
-  </si>
-  <si>
-    <t>Милева</t>
-  </si>
-  <si>
     <t>Атанас</t>
   </si>
   <si>
@@ -133,9 +120,6 @@
     <t>Илия</t>
   </si>
   <si>
-    <t>Великов</t>
-  </si>
-  <si>
     <t>Мачкърски</t>
   </si>
   <si>
@@ -199,15 +183,6 @@
     <t>Андреев</t>
   </si>
   <si>
-    <t>Мирослав</t>
-  </si>
-  <si>
-    <t>Мирославов</t>
-  </si>
-  <si>
-    <t>Гергинов</t>
-  </si>
-  <si>
     <t>Михаела</t>
   </si>
   <si>
@@ -224,15 +199,6 @@
   </si>
   <si>
     <t>Абрашева</t>
-  </si>
-  <si>
-    <t>Павел</t>
-  </si>
-  <si>
-    <t>Павлов</t>
-  </si>
-  <si>
-    <t>Траянов</t>
   </si>
   <si>
     <t>Петър</t>
@@ -665,10 +631,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8E35486-131C-4B3F-8B65-83A02D70C427}">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -722,21 +688,23 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
-        <v>72113</v>
+        <v>72020</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>13</v>
-      </c>
       <c r="E2" s="5">
         <v>1</v>
       </c>
-      <c r="F2" s="5"/>
+      <c r="F2" s="5">
+        <v>2</v>
+      </c>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
@@ -745,21 +713,23 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
-        <v>72020</v>
+        <v>72018</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E3" s="5">
         <v>1</v>
       </c>
-      <c r="F3" s="5"/>
+      <c r="F3" s="5">
+        <v>5.4</v>
+      </c>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
@@ -768,21 +738,23 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
-        <v>72018</v>
+        <v>72028</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E4" s="5">
         <v>1</v>
       </c>
-      <c r="F4" s="5"/>
+      <c r="F4" s="5">
+        <v>5.6</v>
+      </c>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
@@ -791,21 +763,23 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
-        <v>81572</v>
+        <v>72029</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E5" s="5">
         <v>1</v>
       </c>
-      <c r="F5" s="5"/>
+      <c r="F5" s="5">
+        <v>5.4</v>
+      </c>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
@@ -814,21 +788,23 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
-        <v>72028</v>
+        <v>72026</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="E6" s="5">
         <v>1</v>
       </c>
-      <c r="F6" s="5"/>
+      <c r="F6" s="5">
+        <v>3.75</v>
+      </c>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
@@ -837,21 +813,23 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
-        <v>72029</v>
+        <v>72025</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E7" s="5">
         <v>1</v>
       </c>
-      <c r="F7" s="5"/>
+      <c r="F7" s="5">
+        <v>5.5</v>
+      </c>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
@@ -860,21 +838,23 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
-        <v>72026</v>
+        <v>182</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="E8" s="5">
         <v>1</v>
       </c>
-      <c r="F8" s="5"/>
+      <c r="F8" s="5">
+        <v>5.25</v>
+      </c>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
@@ -883,13 +863,13 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
-        <v>72025</v>
+        <v>72034</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>31</v>
@@ -897,7 +877,9 @@
       <c r="E9" s="5">
         <v>1</v>
       </c>
-      <c r="F9" s="5"/>
+      <c r="F9" s="5">
+        <v>3.5</v>
+      </c>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
@@ -906,21 +888,23 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
-        <v>182</v>
+        <v>72019</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>32</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E10" s="5">
         <v>1</v>
       </c>
-      <c r="F10" s="5"/>
+      <c r="F10" s="5">
+        <v>2</v>
+      </c>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
@@ -929,21 +913,23 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
-        <v>72017</v>
+        <v>72016</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E11" s="5">
         <v>1</v>
       </c>
-      <c r="F11" s="5"/>
+      <c r="F11" s="5">
+        <v>5.95</v>
+      </c>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
@@ -952,21 +938,23 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
-        <v>72034</v>
+        <v>72104</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E12" s="5">
         <v>1</v>
       </c>
-      <c r="F12" s="5"/>
+      <c r="F12" s="5">
+        <v>2</v>
+      </c>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
@@ -975,21 +963,23 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
-        <v>72019</v>
+        <v>72013</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="E13" s="5">
         <v>1</v>
       </c>
-      <c r="F13" s="5"/>
+      <c r="F13" s="5">
+        <v>6</v>
+      </c>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
@@ -998,21 +988,23 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
-        <v>72016</v>
+        <v>72015</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="E14" s="5">
         <v>1</v>
       </c>
-      <c r="F14" s="5"/>
+      <c r="F14" s="5">
+        <v>5.95</v>
+      </c>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
@@ -1021,21 +1013,23 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
-        <v>72104</v>
+        <v>72021</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E15" s="5">
         <v>1</v>
       </c>
-      <c r="F15" s="5"/>
+      <c r="F15" s="5">
+        <v>6</v>
+      </c>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
@@ -1044,21 +1038,23 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
-        <v>72013</v>
+        <v>72024</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E16" s="5">
         <v>1</v>
       </c>
-      <c r="F16" s="5"/>
+      <c r="F16" s="5">
+        <v>2</v>
+      </c>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
@@ -1067,21 +1063,23 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
-        <v>72015</v>
+        <v>72030</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="E17" s="5">
         <v>1</v>
       </c>
-      <c r="F17" s="5"/>
+      <c r="F17" s="5">
+        <v>4.95</v>
+      </c>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
@@ -1090,21 +1088,23 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
-        <v>72021</v>
+        <v>72033</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E18" s="5">
         <v>1</v>
       </c>
-      <c r="F18" s="5"/>
+      <c r="F18" s="5">
+        <v>6</v>
+      </c>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
@@ -1113,21 +1113,23 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
-        <v>72024</v>
+        <v>72013</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>55</v>
+        <v>26</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="E19" s="5">
         <v>1</v>
       </c>
-      <c r="F19" s="5"/>
+      <c r="F19" s="5">
+        <v>6</v>
+      </c>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
@@ -1136,21 +1138,23 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
-        <v>72106</v>
+        <v>72014</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E20" s="5">
         <v>1</v>
       </c>
-      <c r="F20" s="5"/>
+      <c r="F20" s="5">
+        <v>5.4</v>
+      </c>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
@@ -1159,21 +1163,23 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="5">
-        <v>72030</v>
+        <v>72032</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E21" s="5">
         <v>1</v>
       </c>
-      <c r="F21" s="5"/>
+      <c r="F21" s="5">
+        <v>6</v>
+      </c>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
@@ -1182,21 +1188,23 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="5">
-        <v>72033</v>
+        <v>72027</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E22" s="5">
         <v>1</v>
       </c>
-      <c r="F22" s="5"/>
+      <c r="F22" s="5">
+        <v>5.7</v>
+      </c>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
@@ -1205,142 +1213,29 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
-        <v>31534</v>
+        <v>72023</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E23" s="5">
         <v>1</v>
       </c>
-      <c r="F23" s="5"/>
+      <c r="F23" s="5">
+        <v>3.5</v>
+      </c>
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
       <c r="K23" s="5"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A24" s="5">
-        <v>72013</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="E24" s="5">
-        <v>1</v>
-      </c>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="5"/>
-      <c r="K24" s="5"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A25" s="5">
-        <v>72014</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="E25" s="5">
-        <v>1</v>
-      </c>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
-      <c r="J25" s="5"/>
-      <c r="K25" s="5"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A26" s="5">
-        <v>72032</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="E26" s="5">
-        <v>1</v>
-      </c>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
-      <c r="I26" s="5"/>
-      <c r="J26" s="5"/>
-      <c r="K26" s="5"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A27" s="5">
-        <v>72027</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="E27" s="5">
-        <v>1</v>
-      </c>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
-      <c r="H27" s="5"/>
-      <c r="I27" s="5"/>
-      <c r="J27" s="5"/>
-      <c r="K27" s="5"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A28" s="5">
-        <v>72023</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="E28" s="5">
-        <v>1</v>
-      </c>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
-      <c r="H28" s="5"/>
-      <c r="I28" s="5"/>
-      <c r="J28" s="5"/>
-      <c r="K28" s="5"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>